<commit_message>
update add file with validate to DB
</commit_message>
<xml_diff>
--- a/Resource/TestExcel/TestExcel.xlsx
+++ b/Resource/TestExcel/TestExcel.xlsx
@@ -1,41 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtnghia\Documents\GitHub\CukCuk-G-2\Resource\TestExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\MISA-CukCuk-Duplicate\Resource\TestExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BC54E9-8223-4384-92B8-53CF3A61C87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D43E5D-E0AE-4B8E-8A23-BDC0EB4DF6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E032AE7C-7CB2-4D49-BBEC-605C9B1576C3}"/>
+    <workbookView xWindow="3900" yWindow="2910" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Mã Nguyên vật liệu</t>
+  </si>
   <si>
     <t>Tên nguyên vật liệu</t>
   </si>
@@ -52,100 +45,16 @@
     <t>BH-60817</t>
   </si>
   <si>
-    <t>BH-60814</t>
-  </si>
-  <si>
-    <t>BH-60813</t>
-  </si>
-  <si>
-    <t>BH-60811</t>
-  </si>
-  <si>
-    <t>BH-60819</t>
-  </si>
-  <si>
-    <t>Bia Hơi</t>
-  </si>
-  <si>
-    <t>Bia không cồn</t>
-  </si>
-  <si>
-    <t>Bia Đức</t>
-  </si>
-  <si>
-    <t>Bia Pháp</t>
-  </si>
-  <si>
-    <t>Bia Sài Gòn</t>
-  </si>
-  <si>
-    <t>Bia Hà Nội</t>
-  </si>
-  <si>
-    <t>Chai</t>
-  </si>
-  <si>
-    <t>Két</t>
-  </si>
-  <si>
-    <t>Hello world</t>
-  </si>
-  <si>
-    <t>Hello world1</t>
-  </si>
-  <si>
-    <t>Hello world3</t>
-  </si>
-  <si>
-    <t>Hello world5</t>
-  </si>
-  <si>
-    <t>Hello world7</t>
-  </si>
-  <si>
-    <t>Hello world8</t>
-  </si>
-  <si>
-    <t>Nhóm 1</t>
-  </si>
-  <si>
-    <t>Nhóm 2</t>
-  </si>
-  <si>
-    <t>Nhóm 3</t>
-  </si>
-  <si>
-    <t>Nhóm 4</t>
-  </si>
-  <si>
-    <t>Nhóm 5</t>
-  </si>
-  <si>
-    <t>Nhóm 7</t>
-  </si>
-  <si>
-    <t>Nhóm 9</t>
-  </si>
-  <si>
-    <t>Mã nguyên v?t li?u</t>
-  </si>
-  <si>
-    <t>Nh?p kh?u</t>
-  </si>
-  <si>
-    <t>BH-60812</t>
-  </si>
-  <si>
-    <t>Bia Tươi</t>
-  </si>
-  <si>
-    <t>Bia Tốt</t>
-  </si>
-  <si>
-    <t>Bia Đan Mạch</t>
-  </si>
-  <si>
-    <t>F-60815</t>
+    <t>Nhập khẩu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhóm 1 </t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Bia tươi</t>
   </si>
 </sst>
 </file>
@@ -233,7 +142,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -245,7 +154,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -292,23 +201,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -344,23 +236,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -512,179 +387,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B88E1B-B12D-4575-88BC-A0F6C618A5C3}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>